<commit_message>
Move *.xlsx to resources folder
</commit_message>
<xml_diff>
--- a/resources/Easy_output.xlsx
+++ b/resources/Easy_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="208">
   <si>
     <t>Nouns</t>
   </si>
@@ -415,7 +415,7 @@
     <t>slow</t>
   </si>
   <si>
-    <t>dad</t>
+    <t>brother</t>
   </si>
   <si>
     <t>hot</t>
@@ -424,7 +424,7 @@
     <t>come</t>
   </si>
   <si>
-    <t>brother</t>
+    <t>child</t>
   </si>
   <si>
     <t>wet</t>
@@ -433,7 +433,7 @@
     <t>make</t>
   </si>
   <si>
-    <t>child</t>
+    <t>area</t>
   </si>
   <si>
     <t>empty</t>
@@ -442,7 +442,7 @@
     <t>run</t>
   </si>
   <si>
-    <t>area</t>
+    <t>corner</t>
   </si>
   <si>
     <t>full</t>
@@ -451,7 +451,7 @@
     <t>jump</t>
   </si>
   <si>
-    <t>corner</t>
+    <t>college</t>
   </si>
   <si>
     <t>fat</t>
@@ -460,7 +460,7 @@
     <t>walk</t>
   </si>
   <si>
-    <t>college</t>
+    <t>bus</t>
   </si>
   <si>
     <t>hard</t>
@@ -469,7 +469,7 @@
     <t>lose</t>
   </si>
   <si>
-    <t>bus</t>
+    <t>boat</t>
   </si>
   <si>
     <t>nice</t>
@@ -478,7 +478,7 @@
     <t>win</t>
   </si>
   <si>
-    <t>boat</t>
+    <t>bag</t>
   </si>
   <si>
     <t>beautiful</t>
@@ -487,7 +487,7 @@
     <t>have</t>
   </si>
   <si>
-    <t>bag</t>
+    <t>car</t>
   </si>
   <si>
     <t>dark</t>
@@ -496,7 +496,7 @@
     <t>see</t>
   </si>
   <si>
-    <t>car</t>
+    <t>answer</t>
   </si>
   <si>
     <t>fun</t>
@@ -505,7 +505,7 @@
     <t>want</t>
   </si>
   <si>
-    <t>answer</t>
+    <t>body</t>
   </si>
   <si>
     <t>long</t>
@@ -514,7 +514,7 @@
     <t>hit</t>
   </si>
   <si>
-    <t>body</t>
+    <t>brain</t>
   </si>
   <si>
     <t>important</t>
@@ -523,7 +523,7 @@
     <t>sleep</t>
   </si>
   <si>
-    <t>brain</t>
+    <t>arm</t>
   </si>
   <si>
     <t>good</t>
@@ -532,7 +532,7 @@
     <t>help</t>
   </si>
   <si>
-    <t>arm</t>
+    <t>blood</t>
   </si>
   <si>
     <t>ready</t>
@@ -541,91 +541,85 @@
     <t>show</t>
   </si>
   <si>
-    <t>blood</t>
+    <t>America</t>
   </si>
   <si>
     <t>hear</t>
   </si>
   <si>
-    <t>America</t>
+    <t>uncle</t>
   </si>
   <si>
     <t>play</t>
   </si>
   <si>
-    <t>uncle</t>
+    <t>sister</t>
   </si>
   <si>
     <t>happen</t>
   </si>
   <si>
-    <t>sister</t>
+    <t>milk</t>
   </si>
   <si>
     <t>stand</t>
   </si>
   <si>
-    <t>mom</t>
+    <t>cookie</t>
   </si>
   <si>
     <t>read</t>
   </si>
   <si>
-    <t>milk</t>
+    <t>apple</t>
   </si>
   <si>
     <t>remember</t>
   </si>
   <si>
-    <t>cookie</t>
+    <t>tree</t>
   </si>
   <si>
     <t>open</t>
   </si>
   <si>
-    <t>apple</t>
+    <t>bush</t>
   </si>
   <si>
     <t>teach</t>
   </si>
   <si>
-    <t>tree</t>
+    <t>flower</t>
   </si>
   <si>
     <t>build</t>
   </si>
   <si>
-    <t>bush</t>
+    <t>leaf</t>
   </si>
   <si>
     <t>eat</t>
   </si>
   <si>
-    <t>flower</t>
+    <t>dirt</t>
   </si>
   <si>
     <t>drink</t>
   </si>
   <si>
-    <t>leaf</t>
-  </si>
-  <si>
     <t>like</t>
   </si>
   <si>
-    <t>dirt</t>
+    <t>leg</t>
   </si>
   <si>
     <t>get</t>
   </si>
   <si>
+    <t>potato</t>
+  </si>
+  <si>
     <t>say</t>
-  </si>
-  <si>
-    <t>leg</t>
-  </si>
-  <si>
-    <t>potato</t>
   </si>
   <si>
     <t>head</t>
@@ -980,7 +974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1025,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1858,11 +1852,11 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="B59" t="s"/>
       <c r="C59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D59" t="s"/>
       <c r="E59" t="s"/>
@@ -1870,11 +1864,11 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B60" t="s"/>
       <c r="C60" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D60" t="s"/>
       <c r="E60" t="s"/>
@@ -1882,7 +1876,7 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="B61" t="s"/>
       <c r="C61" t="s">
@@ -1934,7 +1928,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="B66" t="s"/>
       <c r="C66" t="s"/>
@@ -1944,7 +1938,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B67" t="s"/>
       <c r="C67" t="s"/>
@@ -1954,7 +1948,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="B68" t="s"/>
       <c r="C68" t="s"/>
@@ -1962,26 +1956,6 @@
       <c r="E68" t="s"/>
       <c r="F68" t="s"/>
     </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
-        <v>208</v>
-      </c>
-      <c r="B69" t="s"/>
-      <c r="C69" t="s"/>
-      <c r="D69" t="s"/>
-      <c r="E69" t="s"/>
-      <c r="F69" t="s"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
-        <v>209</v>
-      </c>
-      <c r="B70" t="s"/>
-      <c r="C70" t="s"/>
-      <c r="D70" t="s"/>
-      <c r="E70" t="s"/>
-      <c r="F70" t="s"/>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>